<commit_message>
Add engimon xlsx sample
</commit_message>
<xml_diff>
--- a/input/Engimon.xlsx
+++ b/input/Engimon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STEI\Sem4\PBO\Tubes2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F5131E-4295-438F-B854-8FF854404A36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B373C009-3A16-4AE3-983F-CD5D565F27FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2220F236-1362-4FC8-8C2A-8F31A1E32F85}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>FIRE</t>
   </si>
   <si>
-    <t>Flamethrower</t>
-  </si>
-  <si>
     <t>Ice Beam</t>
   </si>
   <si>
@@ -69,16 +66,496 @@
     <t>Response 2</t>
   </si>
   <si>
-    <t>Ember bocorrr</t>
-  </si>
-  <si>
-    <t>Bocor bocor</t>
-  </si>
-  <si>
-    <t>HAHAHAHA</t>
-  </si>
-  <si>
-    <t>HEHEHEHE</t>
+    <t>Brrr..</t>
+  </si>
+  <si>
+    <t>Ron! Ron!!</t>
+  </si>
+  <si>
+    <t>Hail! Hail!!</t>
+  </si>
+  <si>
+    <t>Loon..</t>
+  </si>
+  <si>
+    <t>Fire Pledge</t>
+  </si>
+  <si>
+    <t>Soliust</t>
+  </si>
+  <si>
+    <t>GROUND</t>
+  </si>
+  <si>
+    <t>Body Slam</t>
+  </si>
+  <si>
+    <t>Grust..</t>
+  </si>
+  <si>
+    <t>Loouuust</t>
+  </si>
+  <si>
+    <t>Bulbmon</t>
+  </si>
+  <si>
+    <t>ELECTRIC</t>
+  </si>
+  <si>
+    <t>Thunderbolt</t>
+  </si>
+  <si>
+    <t>Bulbo, bulbo!</t>
+  </si>
+  <si>
+    <t>I need electricity</t>
+  </si>
+  <si>
+    <t>Aquaron</t>
+  </si>
+  <si>
+    <t>WATER</t>
+  </si>
+  <si>
+    <t>Water Pledge</t>
+  </si>
+  <si>
+    <t>Aqua qua qua</t>
+  </si>
+  <si>
+    <t>Quda quda quda</t>
+  </si>
+  <si>
+    <t>Sparkymon</t>
+  </si>
+  <si>
+    <t>Fire Blast</t>
+  </si>
+  <si>
+    <t>Sparky parky!</t>
+  </si>
+  <si>
+    <t>Party parky!</t>
+  </si>
+  <si>
+    <t>Icypicy</t>
+  </si>
+  <si>
+    <t>Ice Hammer</t>
+  </si>
+  <si>
+    <t>cyp cyp</t>
+  </si>
+  <si>
+    <t>icy icy</t>
+  </si>
+  <si>
+    <t>CacingAlaska</t>
+  </si>
+  <si>
+    <t>Bull Doze</t>
+  </si>
+  <si>
+    <t>Dimana spongebob?</t>
+  </si>
+  <si>
+    <t>Saya perlu nanas laut</t>
+  </si>
+  <si>
+    <t>Chupika</t>
+  </si>
+  <si>
+    <t>Shock Wave</t>
+  </si>
+  <si>
+    <t>Chupi, chupii</t>
+  </si>
+  <si>
+    <t>Piii..</t>
+  </si>
+  <si>
+    <t>Flooduf</t>
+  </si>
+  <si>
+    <t>Liquidation</t>
+  </si>
+  <si>
+    <t>loo looo</t>
+  </si>
+  <si>
+    <t>loooooduffff</t>
+  </si>
+  <si>
+    <t>Coldhell</t>
+  </si>
+  <si>
+    <t>FIRE,ICE</t>
+  </si>
+  <si>
+    <t>Freezing Flame</t>
+  </si>
+  <si>
+    <t>The hell is freezing…</t>
+  </si>
+  <si>
+    <t>There's global warming in hell, do you even know that?</t>
+  </si>
+  <si>
+    <t>Magmatuar</t>
+  </si>
+  <si>
+    <t>FIRE,GROUND</t>
+  </si>
+  <si>
+    <t>Magma is very hot, yet very relaxing</t>
+  </si>
+  <si>
+    <t>Magmatuarrrrr!!!</t>
+  </si>
+  <si>
+    <t>Electrosion</t>
+  </si>
+  <si>
+    <t>FIRE,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Thunder Blast</t>
+  </si>
+  <si>
+    <t>Troooooo…</t>
+  </si>
+  <si>
+    <t>PAR sangat susah</t>
+  </si>
+  <si>
+    <t>Sealame</t>
+  </si>
+  <si>
+    <t>FIRE,WATER</t>
+  </si>
+  <si>
+    <t>Double Edge</t>
+  </si>
+  <si>
+    <t>Siiiie..</t>
+  </si>
+  <si>
+    <t>Fire and water is not a good idea</t>
+  </si>
+  <si>
+    <t>Antartic</t>
+  </si>
+  <si>
+    <t>ICE,GROUND</t>
+  </si>
+  <si>
+    <t>Avalanche</t>
+  </si>
+  <si>
+    <t>Tiiic, tiii..</t>
+  </si>
+  <si>
+    <t>My homeland.. Is disappearing</t>
+  </si>
+  <si>
+    <t>Culcas</t>
+  </si>
+  <si>
+    <t>ICE,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Cold Refrigerator</t>
+  </si>
+  <si>
+    <t>2 Pintu lebih baik dari 1 pintu</t>
+  </si>
+  <si>
+    <t>Casss… Culcassss!</t>
+  </si>
+  <si>
+    <t>Labile</t>
+  </si>
+  <si>
+    <t>ICE,WATER</t>
+  </si>
+  <si>
+    <t>Biiii..</t>
+  </si>
+  <si>
+    <t>Bilbilbiiiiiii..</t>
+  </si>
+  <si>
+    <t>Gustmon</t>
+  </si>
+  <si>
+    <t>GROUND,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Tectonic Rage</t>
+  </si>
+  <si>
+    <t>Gusti apa ini</t>
+  </si>
+  <si>
+    <t>Gust guusst!</t>
+  </si>
+  <si>
+    <t>Trenchmon</t>
+  </si>
+  <si>
+    <t>GROUND,WATER</t>
+  </si>
+  <si>
+    <t>Giga Impact</t>
+  </si>
+  <si>
+    <t>Mariana trench is deeper than you think!</t>
+  </si>
+  <si>
+    <t>Trenchy, trenchy!</t>
+  </si>
+  <si>
+    <t>Voltense</t>
+  </si>
+  <si>
+    <t>ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>Korslet</t>
+  </si>
+  <si>
+    <t>PLN belum bayar</t>
+  </si>
+  <si>
+    <t>Token listrik memusnahkan saya</t>
+  </si>
+  <si>
+    <t>Ficigmon</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,GROUND</t>
+  </si>
+  <si>
+    <t>Ficiii</t>
+  </si>
+  <si>
+    <t>Is this digimon??</t>
+  </si>
+  <si>
+    <t>Circogord</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Cirrr</t>
+  </si>
+  <si>
+    <t>Cooo</t>
+  </si>
+  <si>
+    <t>Icify</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,WATER</t>
+  </si>
+  <si>
+    <t>Burning Chill</t>
+  </si>
+  <si>
+    <t>Brrrrr</t>
+  </si>
+  <si>
+    <t>BRRRRRR</t>
+  </si>
+  <si>
+    <t>LoveMagama</t>
+  </si>
+  <si>
+    <t>FIRE,GROUND,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Steam Bomb</t>
+  </si>
+  <si>
+    <t>Lovee some magama</t>
+  </si>
+  <si>
+    <t>who is magama</t>
+  </si>
+  <si>
+    <t>Tetonicy</t>
+  </si>
+  <si>
+    <t>FIRE,GROUND,WATER</t>
+  </si>
+  <si>
+    <t>Mudflood</t>
+  </si>
+  <si>
+    <t>Tekto, tektooo!</t>
+  </si>
+  <si>
+    <t>I can make the whole ground shaking, that's called tectonic!</t>
+  </si>
+  <si>
+    <t>PerfectDisaster</t>
+  </si>
+  <si>
+    <t>FIRE,ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>Shock and Burn</t>
+  </si>
+  <si>
+    <t>covid vid vid</t>
+  </si>
+  <si>
+    <t>nubes tubes lagi tubes</t>
+  </si>
+  <si>
+    <t>Iglosify</t>
+  </si>
+  <si>
+    <t>ICE,GROUND,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Weather Ball</t>
+  </si>
+  <si>
+    <t>cuaca hari ini</t>
+  </si>
+  <si>
+    <t>terang benderang</t>
+  </si>
+  <si>
+    <t>Trofii</t>
+  </si>
+  <si>
+    <t>ICE,GROUND,WATER</t>
+  </si>
+  <si>
+    <t>Muddy Water</t>
+  </si>
+  <si>
+    <t>trolilili</t>
+  </si>
+  <si>
+    <t>fuuuuulingggg</t>
+  </si>
+  <si>
+    <t>Syverter</t>
+  </si>
+  <si>
+    <t>ICE,ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>vert verttt</t>
+  </si>
+  <si>
+    <t>kentut bunyinya pret</t>
+  </si>
+  <si>
+    <t>Oonga</t>
+  </si>
+  <si>
+    <t>GROUND,ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>Eruption</t>
+  </si>
+  <si>
+    <t>oonga oonga</t>
+  </si>
+  <si>
+    <t>ngaoo ngaoo</t>
+  </si>
+  <si>
+    <t>Hokkien</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,GROUND,ELECTRIC</t>
+  </si>
+  <si>
+    <t>Earth Power</t>
+  </si>
+  <si>
+    <t>hok hok hok</t>
+  </si>
+  <si>
+    <t>ki ki ki &gt;.&lt;!</t>
+  </si>
+  <si>
+    <t>Arleen</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,GROUND,WATER</t>
+  </si>
+  <si>
+    <t>Melt the Ground</t>
+  </si>
+  <si>
+    <t>aldi is here</t>
+  </si>
+  <si>
+    <t>arrrrrr….lennn</t>
+  </si>
+  <si>
+    <t>Maxeew</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>aduh aduh aduh</t>
+  </si>
+  <si>
+    <t>ez ez ez</t>
+  </si>
+  <si>
+    <t>Shijeew</t>
+  </si>
+  <si>
+    <t>FIRE,GROUND,ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>Lava Plume</t>
+  </si>
+  <si>
+    <t>jeew strongg!</t>
+  </si>
+  <si>
+    <t>shishishi</t>
+  </si>
+  <si>
+    <t>Pegow</t>
+  </si>
+  <si>
+    <t>Freeze Dry</t>
+  </si>
+  <si>
+    <t>gope gope gope</t>
+  </si>
+  <si>
+    <t>cepe cepe cepe</t>
+  </si>
+  <si>
+    <t>Frederon</t>
+  </si>
+  <si>
+    <t>FIRE,ICE,GROUND,ELECTRIC,WATER</t>
+  </si>
+  <si>
+    <t>Godly Fart</t>
+  </si>
+  <si>
+    <t>hehe haha</t>
+  </si>
+  <si>
+    <t>hoho huhu</t>
   </si>
 </sst>
 </file>
@@ -430,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAA2AB0-BD4B-4942-9DAC-0BAE7234D902}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +933,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -470,30 +947,608 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>